<commit_message>
- added note to unit test
- fix https://github.com/ClosedXML/ClosedXML/issues/1575
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/TryToLoad/ThreadedComment.xlsx
+++ b/ClosedXML.Tests/Resource/TryToLoad/ThreadedComment.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="202300"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5321D3A6-B66F-4C4A-9C6F-B18D9A11D09A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB94B8C-AFE2-42BE-8312-DEF2F3A4ECA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{A59FA85D-AC97-4E90-8C7A-CEA236BD4406}"/>
   </bookViews>
@@ -34,6 +34,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={49C52447-16DF-491E-8BD1-273F700714C6}</author>
+    <author>Author</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{49C52447-16DF-491E-8BD1-273F700714C6}">
@@ -46,21 +47,48 @@
     This is a reply.</t>
       </text>
     </comment>
+    <comment ref="A2" authorId="1" shapeId="0" xr:uid="{99B089E6-C2C6-4559-A2B1-F2151A22F82F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+A note</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>This cell has a threaded comment</t>
   </si>
+  <si>
+    <t>This cell has a note</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -69,6 +97,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
@@ -112,10 +147,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -446,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18918452-643D-4B0C-846C-EDD5AAB4F92E}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -462,6 +493,11 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>